<commit_message>
Add CTDC static data verifications and minor fixes
</commit_message>
<xml_diff>
--- a/InputFiles/C3DC/C3DC_StaticData.xlsx
+++ b/InputFiles/C3DC/C3DC_StaticData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git/Commons_Automation/InputFiles/C3DC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB7CC15-3DFF-0E49-900D-62B8BA963EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9744E084-76CD-6040-98A3-0ED323A62E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4100" yWindow="3820" windowWidth="31900" windowHeight="18140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V_HomePage" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="116">
   <si>
     <t>verificationText</t>
   </si>
@@ -166,9 +166,6 @@
     <t>FooterAboutCCDILink</t>
   </si>
   <si>
-    <t>FooterAboutContactCCDILink</t>
-  </si>
-  <si>
     <t>FooterResourcesC3DCLink</t>
   </si>
   <si>
@@ -208,9 +205,6 @@
     <t>About CCDI</t>
   </si>
   <si>
-    <t>Contact CCDI</t>
-  </si>
-  <si>
     <t>C3DC Data Model</t>
   </si>
   <si>
@@ -247,9 +241,6 @@
     <t>ncichildhoodcancerdatainitiative@mail.nih.gov</t>
   </si>
   <si>
-    <t>Childhood Cancer Data Initiative The NCI’s Childhood Cancer Data Initiative (CCDI), which the Childhood Cancer Clinical Data Commons is part of, is an initiative seeking to build a community centered around childhood cancer care and research. Through enhanced data sharing, the initiative works to improve understanding of cancer biology, preventive measures, treatment, quality of life, and survivorship, as well as ensure that the community can learn from every child with cancer. Sign-up for email updates from NCI about CCDI.</t>
-  </si>
-  <si>
     <t>Childhood Cancer Clinical Data Commons The Childhood Cancer Clinical Data Commons (C3DC) is an open-access web application that serves as the primary source for deidentified, individual-level harmonized data that describes the demographic and phenotypic characteristics of participants. This harmonization process uses a standard data dictionary consisting of Common Data Elements (CDEs), C3DC employs a common data model to facilitate cohort analyses and correlative analytics with data in other datatype-specific commons.The data model has been deposited in GitHub.</t>
   </si>
   <si>
@@ -343,9 +334,6 @@
     <t>ResourcesTitle</t>
   </si>
   <si>
-    <t>Questions for C3DC? The Childhood Cancer Data Initiative (CCDI) welcomes community input to improve this web application usability. Please send your feedback and suggestions to ncichildhoodcancerdatainitiative@mail.nih.gov.Your contributions are valuable to enhancing the user experience.</t>
-  </si>
-  <si>
     <t>A GROWING RESOURCE NETWORK</t>
   </si>
   <si>
@@ -362,6 +350,27 @@
   </si>
   <si>
     <t>caDSR The Cancer Data Standards Repository is one of the largest CDE registries developed by the National Cancer Institute (NCI) and contains over 75,000 CDEs covering many aspects of cancer research. Access it here: https://cadsr.cancer.gov/onedata/Home.jsp. There are over 400 pediatric CDEs used by various entities like CCDI Data Ecosystem and Pediatric Clinical Data commons. The CCDI Pediatric Cancer Core Common Data Elements (CDEs) were created to standardize data collection and sharing for pediatric cancer research. To explore these standards, visit the caDSR homepage and select "Pediatric Cancer Core CDEs" under the Favorites column for a custom report of key CDEs. For feedback or suggestions, email the CCDI mailbox.</t>
+  </si>
+  <si>
+    <t>Questions for C3DC? The Childhood Cancer Data Initiative (CCDI) welcomes community input to improve this web application usability. Please send your feedback and suggestions to ncichildhoodcancerdatainitiative@mail.nih.gov. Your contributions are valuable to enhancing the user experience.</t>
+  </si>
+  <si>
+    <t>Childhood Cancer Data Initiative The NCI’s Childhood Cancer Data Initiative (CCDI), which the Childhood Cancer Clinical Data Commons is part of, is an initiative seeking to build a community centered around childhood cancer care and research. Through enhanced data sharing, the initiative works to improve understanding of cancer biology, preventive measures, treatment, quality of life, and survivorship, as well as ensure that the community can learn from every child with cancer. C3DC is part of the CCDI Data Ecosystem. Learn more about other CCDI data and resources on the CCDI Hub. Sign-up for email updates from NCI about CCDI.</t>
+  </si>
+  <si>
+    <t>FooterAboutContactUsLink</t>
+  </si>
+  <si>
+    <t>Contact Us</t>
+  </si>
+  <si>
+    <t>FooterAboutReleaseNotesLink</t>
+  </si>
+  <si>
+    <t>https://clinicalcommons-qa.ccdi.cancer.gov/release_notes_pdf</t>
+  </si>
+  <si>
+    <t>Release Notes</t>
   </si>
 </sst>
 </file>
@@ -455,7 +464,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -487,6 +496,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -706,10 +718,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -727,7 +739,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -812,7 +824,7 @@
     </row>
     <row r="12" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>10</v>
@@ -823,10 +835,10 @@
         <v>45</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -834,7 +846,7 @@
         <v>46</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>11</v>
@@ -842,105 +854,116 @@
     </row>
     <row r="15" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>13</v>
+        <v>113</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>15</v>
+        <v>60</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>16</v>
+        <v>61</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>18</v>
+        <v>62</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C24" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -949,13 +972,15 @@
     <hyperlink ref="C13" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="C14" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="C15" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C17" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C20" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C21" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="C22" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="C23" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="C24" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="C18" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C18" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C21" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C22" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C23" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C24" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C25" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C19" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B15" r:id="rId11" display="mailto:NCIChildhoodCancerDataInitiative@mail.nih.gov" xr:uid="{31D0942C-20C4-C040-973D-71CFF4D90535}"/>
+    <hyperlink ref="C16" r:id="rId12" xr:uid="{F5A6731B-1C0A-4A4B-A314-3AEEB744F756}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -987,12 +1012,12 @@
         <v>0</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>31</v>
@@ -1000,7 +1025,7 @@
     </row>
     <row r="3" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>32</v>
@@ -1008,7 +1033,7 @@
     </row>
     <row r="4" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>4</v>
@@ -1019,10 +1044,10 @@
     </row>
     <row r="5" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>29</v>
@@ -1063,20 +1088,20 @@
         <v>0</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="9" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>25</v>
@@ -1084,47 +1109,47 @@
     </row>
     <row r="4" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>14</v>
@@ -1135,7 +1160,7 @@
     </row>
     <row r="10" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>26</v>
@@ -1146,7 +1171,7 @@
     </row>
     <row r="11" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>27</v>
@@ -1157,7 +1182,7 @@
     </row>
     <row r="12" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>28</v>
@@ -1168,7 +1193,7 @@
     </row>
     <row r="13" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>29</v>
@@ -1179,10 +1204,10 @@
     </row>
     <row r="14" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>30</v>
@@ -1209,8 +1234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EFF1735-A88B-8349-987A-9071787E8819}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1228,51 +1253,51 @@
         <v>0</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="70" x14ac:dyDescent="0.15">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>74</v>
+        <v>110</v>
       </c>
       <c r="C2" s="7"/>
     </row>
     <row r="3" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C3" s="7"/>
     </row>
     <row r="4" spans="1:3" ht="42" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3" ht="42" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>11</v>
@@ -1280,10 +1305,10 @@
     </row>
     <row r="7" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>22</v>
@@ -1291,10 +1316,10 @@
     </row>
     <row r="8" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>23</v>
@@ -1302,10 +1327,10 @@
     </row>
     <row r="9" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>14</v>
@@ -1313,10 +1338,10 @@
     </row>
     <row r="10" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Add About page locators and fixes for homepage locators
</commit_message>
<xml_diff>
--- a/InputFiles/C3DC/C3DC_StaticData.xlsx
+++ b/InputFiles/C3DC/C3DC_StaticData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git/Commons_Automation/InputFiles/C3DC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9744E084-76CD-6040-98A3-0ED323A62E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24215262-2212-B149-A81F-EB496EADB1F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4100" yWindow="3820" windowWidth="31900" windowHeight="18140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12820" yWindow="-27140" windowWidth="31900" windowHeight="18140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V_HomePage" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="124">
   <si>
     <t>verificationText</t>
   </si>
@@ -371,13 +371,38 @@
   </si>
   <si>
     <t>Release Notes</t>
+  </si>
+  <si>
+    <t>AboutParagraph5</t>
+  </si>
+  <si>
+    <t>Citing the C3DC
+NCI expects users to acknowledge CCDI data use as follows:</t>
+  </si>
+  <si>
+    <t>AboutParagraph6</t>
+  </si>
+  <si>
+    <t>AboutParagraph7</t>
+  </si>
+  <si>
+    <t>AboutParagraph8</t>
+  </si>
+  <si>
+    <t>"The results published here are, in whole or in part, derived from the analysis of data listed in the C3DC (clinicalcommons.ccdi.cancer.gov), established by the National Cancer Institute’s Childhood Cancer Data Initiative (CCDI)."</t>
+  </si>
+  <si>
+    <t>To cite individual studies, note the CCDI study ID (e.g., phs002790) and include the name and URL or link for the C3DC (clinicalcommons.ccdi.cancer.gov), along with the phrase, "established by the National Cancer Institute’s Childhood Cancer Data Initiative (CCDI)."</t>
+  </si>
+  <si>
+    <t>Example: "The results analyzed and &lt;published or shown&gt; here are based in whole or in part from analyzing the Molecular Characterization Initiative data listed in the C3DC (clinicalcommons.ccdi.cancer.gov) under study ID phs002790. The data were accessed from the NCI’s Cancer Research Data Commons (datacommons.cancer.gov). The C3DC was established by the National Cancer Institute’s Childhood Cancer Data Initiative (CCDI)".</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -438,6 +463,12 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -720,7 +751,7 @@
   </sheetPr>
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+    <sheetView zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -1232,10 +1263,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EFF1735-A88B-8349-987A-9071787E8819}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1292,69 +1323,106 @@
       </c>
       <c r="C5" s="7"/>
     </row>
-    <row r="6" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+        <v>116</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+        <v>118</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" spans="1:3" ht="42" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+        <v>119</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>14</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="7"/>
     </row>
     <row r="10" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A14" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B14" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1" xr:uid="{239A22FE-34DA-EA40-A944-3B1D267EAE79}"/>
-    <hyperlink ref="C7" r:id="rId2" xr:uid="{4388C7CF-2A1C-E24B-B270-458EC56FCB6F}"/>
-    <hyperlink ref="C8" r:id="rId3" xr:uid="{26561FE2-58C5-5442-82B4-7FB38D619E48}"/>
-    <hyperlink ref="C10" r:id="rId4" xr:uid="{7E133F14-8719-EE4B-90E8-39CD0E6BF8C5}"/>
-    <hyperlink ref="B10" r:id="rId5" xr:uid="{E0A41BB6-F723-F042-AB8A-D511432535BE}"/>
-    <hyperlink ref="C9" r:id="rId6" xr:uid="{87E132F4-C79C-DC40-80A4-4284605CB15C}"/>
+    <hyperlink ref="C10" r:id="rId1" xr:uid="{239A22FE-34DA-EA40-A944-3B1D267EAE79}"/>
+    <hyperlink ref="C11" r:id="rId2" xr:uid="{4388C7CF-2A1C-E24B-B270-458EC56FCB6F}"/>
+    <hyperlink ref="C12" r:id="rId3" xr:uid="{26561FE2-58C5-5442-82B4-7FB38D619E48}"/>
+    <hyperlink ref="C14" r:id="rId4" xr:uid="{7E133F14-8719-EE4B-90E8-39CD0E6BF8C5}"/>
+    <hyperlink ref="B14" r:id="rId5" xr:uid="{E0A41BB6-F723-F042-AB8A-D511432535BE}"/>
+    <hyperlink ref="C13" r:id="rId6" xr:uid="{87E132F4-C79C-DC40-80A4-4284605CB15C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>